<commit_message>
Added BOM and Gerbers
</commit_message>
<xml_diff>
--- a/Dokumenti/BOM.xlsx
+++ b/Dokumenti/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Nejc Data\Projects\Tabor inovativnih tehnologij\Dokumenti\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Nejc Data\Projects\SummerCampOfInnovativeTechnologies\Dokumenti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3853190B-88AD-4174-973F-29352521578D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCF9F17-D81E-40ED-99F7-B1CF5948902A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2660" yWindow="2660" windowWidth="28800" windowHeight="15500" xr2:uid="{29061E95-3861-4F78-A71A-770A01B038EA}"/>
+    <workbookView xWindow="23800" yWindow="8140" windowWidth="28800" windowHeight="15500" xr2:uid="{29061E95-3861-4F78-A71A-770A01B038EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
   <si>
     <t>Number of parts:</t>
   </si>
@@ -115,15 +115,58 @@
   </si>
   <si>
     <t>MAX:</t>
+  </si>
+  <si>
+    <t>https://si.farnell.com/multicomp/mcwr04x4700ftl/res-470r-1-0-0625w-0402-thick/dp/2447178</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MCWR04X4700FTL</t>
+  </si>
+  <si>
+    <t>100 Ω Resistor</t>
+  </si>
+  <si>
+    <t>Price(100x):</t>
+  </si>
+  <si>
+    <t>SUM:(75)</t>
+  </si>
+  <si>
+    <t>LED Array</t>
+  </si>
+  <si>
+    <t>https://si.farnell.com/lumex/ssa-lxb10hw-gf-lp/bar-graph-10-led-red-4mcd-105mw/dp/1020492?ost=ssa-lxb10hw-gf</t>
+  </si>
+  <si>
+    <t>SSA-LXB10HW-GF/LP..</t>
+  </si>
+  <si>
+    <t>609-4049-1-ND</t>
+  </si>
+  <si>
+    <t>https://si.farnell.com/amphenol-icc-fci/10103593-0001lf/micro-usb-2-0-type-b-receptacle/dp/2293751?ost=609-4049-1-nd&amp;iscrfnonsku=true</t>
+  </si>
+  <si>
+    <t>USB Connector</t>
+  </si>
+  <si>
+    <t>L7805ABD2T-TR</t>
+  </si>
+  <si>
+    <t>Voltage Regulator</t>
+  </si>
+  <si>
+    <t>https://si.farnell.com/stmicroelectronics/l7805abd2t-tr/ic-v-reg-5-0v-d2pak-3-7805/dp/1366571?st=l7805abd2t-tr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-1]"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000\ [$€-1]"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -193,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -208,7 +251,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -223,7 +266,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -238,7 +281,7 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -256,7 +299,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -271,7 +314,7 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -286,21 +329,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -310,13 +338,11 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -325,21 +351,30 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right/>
       <top style="medium">
         <color auto="1"/>
@@ -350,29 +385,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -380,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -392,18 +414,25 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -413,33 +442,19 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -447,28 +462,40 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -784,41 +811,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B3C93E-4727-46D4-B9CF-06DDCFED9428}">
-  <dimension ref="C1:N46"/>
+  <dimension ref="C1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.54296875" customWidth="1"/>
-    <col min="12" max="13" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="99.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="120.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C2" s="32" t="s">
+    <row r="1" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="C2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
       <c r="M2" s="34"/>
-      <c r="N2" s="18"/>
-    </row>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="N2" s="34"/>
+      <c r="O2" s="35"/>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
@@ -847,21 +876,24 @@
         <v>28</v>
       </c>
       <c r="L3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="N3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C4" s="8"/>
       <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="26">
         <v>1</v>
       </c>
       <c r="F4" s="9" t="s">
@@ -885,19 +917,22 @@
       <c r="L4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="24" t="s">
+      <c r="M4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C5" s="11"/>
       <c r="D5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="27">
         <v>2</v>
       </c>
       <c r="F5" s="12" t="s">
@@ -918,24 +953,27 @@
       <c r="K5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="13">
         <f>20*I5*E5</f>
         <v>14.32</v>
       </c>
-      <c r="M5" s="20">
+      <c r="N5" s="19">
         <f>15*I5*E5</f>
         <v>10.74</v>
       </c>
-      <c r="N5" s="21" t="s">
+      <c r="O5" s="20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C6" s="11"/>
       <c r="D6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="27">
         <v>1</v>
       </c>
       <c r="F6" s="12" t="s">
@@ -956,24 +994,27 @@
       <c r="K6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="13">
         <f>20*I6*E6</f>
         <v>11.399999999999999</v>
       </c>
-      <c r="M6" s="20">
+      <c r="N6" s="19">
         <f>15*I6</f>
         <v>8.5499999999999989</v>
       </c>
-      <c r="N6" s="21" t="s">
+      <c r="O6" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C7" s="11"/>
       <c r="D7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="27">
         <v>2</v>
       </c>
       <c r="F7" s="12" t="s">
@@ -994,24 +1035,27 @@
       <c r="K7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="13">
         <f>20*I7*E7</f>
         <v>3.2040000000000002</v>
       </c>
-      <c r="M7" s="20">
+      <c r="N7" s="19">
         <f>15*I7</f>
         <v>1.2015</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="O7" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C8" s="11"/>
       <c r="D8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="27">
         <v>4</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -1032,99 +1076,186 @@
       <c r="K8" s="13">
         <v>0.09</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="13">
         <f>20*K8*E8</f>
         <v>7.1999999999999993</v>
       </c>
-      <c r="M8" s="13" t="e">
-        <f>15*K8*F8</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="13">
+        <f>15*K8*E8</f>
+        <v>5.3999999999999995</v>
+      </c>
+      <c r="O8" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13">
-        <f>20*I9*E9</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="20">
-        <f>15*I9</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="22"/>
-    </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="D9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="27">
+        <v>10</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="30">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="M9" s="13">
+        <f>20*L9*E9</f>
+        <v>0.7400000000000001</v>
+      </c>
+      <c r="N9" s="13">
+        <f>15*L9*E9</f>
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
+      <c r="D10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="27">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="13">
+        <v>2.38</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="13">
+        <v>2.11</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>9</v>
+      </c>
       <c r="L10" s="13">
+        <v>1.4</v>
+      </c>
+      <c r="M10" s="13">
         <f>20*I10*E10</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="20">
-        <f>15*I10</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="22"/>
-    </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.35">
+        <v>42.199999999999996</v>
+      </c>
+      <c r="N10" s="19">
+        <f>15*I10*E10</f>
+        <v>31.65</v>
+      </c>
+      <c r="O10" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13">
+      <c r="D11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="27">
+        <v>1</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="13">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="13">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="13">
         <f>20*I11*E11</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="20">
-        <f>15*I11</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="22"/>
-    </row>
-    <row r="12" spans="3:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>12.1</v>
+      </c>
+      <c r="N11" s="19">
+        <f>15*I11*E11</f>
+        <v>9.0749999999999993</v>
+      </c>
+      <c r="O11" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="13">
+      <c r="D12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="28">
+        <v>1</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="16">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="16">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="13">
         <f>20*I12*E12</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="20">
-        <f>15*I12</f>
-        <v>0</v>
-      </c>
-      <c r="N12" s="23"/>
-    </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.35">
+        <v>13.759999999999998</v>
+      </c>
+      <c r="N12" s="19">
+        <f>15*I12*E12</f>
+        <v>10.319999999999999</v>
+      </c>
+      <c r="O12" s="36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.35">
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1133,8 +1264,9 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.35">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1143,8 +1275,9 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.35">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1153,8 +1286,9 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.35">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1163,8 +1297,9 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.35">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1173,8 +1308,9 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1183,7 +1319,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1192,7 +1328,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1201,7 +1337,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -1210,7 +1346,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -1219,7 +1355,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -1228,7 +1364,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -1237,28 +1373,34 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="D25" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="32">
+        <f>SUM(E4:E24)</f>
+        <v>23</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="25" t="s">
+      <c r="J25" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="K25" s="25"/>
-      <c r="L25" s="26">
-        <f>SUM(L4:L24)</f>
-        <v>36.123999999999995</v>
-      </c>
-      <c r="M25" s="27" t="e">
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="23">
         <f>SUM(M4:M24)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.35">
+        <v>104.92399999999998</v>
+      </c>
+      <c r="N25" s="24">
+        <f>SUM(N4:N24)</f>
+        <v>77.491499999999988</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1266,16 +1408,17 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="25" t="s">
+      <c r="J26" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K26" s="35"/>
-      <c r="L26" s="26">
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="23">
         <f>13*20</f>
         <v>260</v>
       </c>
     </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1284,7 +1427,7 @@
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1293,7 +1436,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1302,7 +1445,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1311,7 +1454,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1320,7 +1463,7 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1439,16 +1582,20 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C2:O2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="N5" r:id="rId1" xr:uid="{26E3C630-BA01-4059-85AE-EF41582FDBB3}"/>
-    <hyperlink ref="N4" r:id="rId2" xr:uid="{5525E9B7-453F-4CDD-B5C8-65ED5F0DB796}"/>
-    <hyperlink ref="N6" r:id="rId3" xr:uid="{95B1591B-DE72-4B53-9FC2-67B6F720D16B}"/>
-    <hyperlink ref="N7" r:id="rId4" xr:uid="{B02B28A7-A51A-415D-BF9C-A460D5D7F510}"/>
-    <hyperlink ref="N8" r:id="rId5" xr:uid="{E684AA05-AB2A-48F9-9AF9-0C35646B824D}"/>
+    <hyperlink ref="O5" r:id="rId1" xr:uid="{26E3C630-BA01-4059-85AE-EF41582FDBB3}"/>
+    <hyperlink ref="O4" r:id="rId2" xr:uid="{5525E9B7-453F-4CDD-B5C8-65ED5F0DB796}"/>
+    <hyperlink ref="O6" r:id="rId3" xr:uid="{95B1591B-DE72-4B53-9FC2-67B6F720D16B}"/>
+    <hyperlink ref="O7" r:id="rId4" xr:uid="{B02B28A7-A51A-415D-BF9C-A460D5D7F510}"/>
+    <hyperlink ref="O8" r:id="rId5" xr:uid="{E684AA05-AB2A-48F9-9AF9-0C35646B824D}"/>
+    <hyperlink ref="O9" r:id="rId6" xr:uid="{B5D36476-7888-4FFE-804F-D8E0D1D272E9}"/>
+    <hyperlink ref="O10" r:id="rId7" xr:uid="{B6646FA9-452C-4330-ACD7-3B39D771313F}"/>
+    <hyperlink ref="O11" r:id="rId8" xr:uid="{225D1BBD-17BF-4310-B6D8-573DC7DC62DF}"/>
+    <hyperlink ref="O12" r:id="rId9" xr:uid="{7FE590D1-068D-4CC8-978E-DF5D4411E0EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>